<commit_message>
WIP FixedConc and FixedAct changes
debugging Donnan Layer problems...
- The FixedAct CompType flag will now actually fix the activity of the component rather than the concentration
- A new FixedConc CompType flag is included for fixing the concentration of a component
- found that the diffusely bound copper is 2 OOM too high compared to the old BLM, so that's where we'll look for problems tomorrow.
</commit_message>
<xml_diff>
--- a/scrap/old BLM/full_organic_SPEC.det.xlsx
+++ b/scrap/old BLM/full_organic_SPEC.det.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kellyc\Documents\BLM Development\engine\BLMEngineInR\scrap\old BLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E9AB3AA-5855-49B8-8F3C-F22E77B2BF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{834F5ACA-0B10-498D-A8C7-2F1CAB9086C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="1116" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="full_organic_SPEC.det" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="124">
-  <si>
-    <t>Ver 3.57.2.50, build 2023-06-15</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="124">
+  <si>
+    <t>Ver 3.57.2.45, build 2021-04-05</t>
   </si>
   <si>
     <t>C:\Program Files (x86)\Biotic Ligand Model - Research Mode\Model\Cu_freshwater_acute_and_chronic_2017-01-17.dat</t>
@@ -145,9 +145,6 @@
     <t>CuHCO3</t>
   </si>
   <si>
-    <t>OH</t>
-  </si>
-  <si>
     <t>TOrg.H</t>
   </si>
   <si>
@@ -166,18 +163,24 @@
     <t>TOrg.K</t>
   </si>
   <si>
-    <t>HA Charge</t>
-  </si>
-  <si>
-    <t>FA Charge</t>
-  </si>
-  <si>
     <t>Charge</t>
   </si>
   <si>
     <t>Ionic S.</t>
   </si>
   <si>
+    <t>Act_z1</t>
+  </si>
+  <si>
+    <t>Act_z2</t>
+  </si>
+  <si>
+    <t>Act_z3</t>
+  </si>
+  <si>
+    <t>Act_z4</t>
+  </si>
+  <si>
     <t>Temp (K)</t>
   </si>
   <si>
@@ -227,9 +230,6 @@
   </si>
   <si>
     <t>mol / kg wet</t>
-  </si>
-  <si>
-    <t>eq / L</t>
   </si>
   <si>
     <t>eq</t>
@@ -467,39 +467,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -551,7 +551,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -662,13 +662,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -677,6 +670,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -741,11 +741,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -755,7 +775,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -935,201 +957,189 @@
         <v>53</v>
       </c>
       <c r="AY5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AZ5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AZ5" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="BA5" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="BB5" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="BC5" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="BD5" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="BE5" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="BF5" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BG5" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="BH5" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="BI5" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="BJ5" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="BK5" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="BL5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="BM5" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:65" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="V6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="W6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="X6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="Y6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S6" s="2" t="s">
+      <c r="Z6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="AA6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="U6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="W6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="X6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA6" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AB6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AG6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AH6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AI6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AJ6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AK6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AM6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AN6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AO6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AP6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AQ6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AR6" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AS6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AT6" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AU6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AV6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AX6" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="AW6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AX6" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="AY6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="BA6" s="2" t="s">
-        <v>73</v>
+      <c r="AZ6" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="BB6" s="2" t="s">
         <v>73</v>
@@ -1162,6 +1172,9 @@
         <v>73</v>
       </c>
       <c r="BL6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="BM6" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1278,43 +1291,43 @@
         <v>1.7560205378686078E-7</v>
       </c>
       <c r="AL7" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>1.0793017642812827E-9</v>
       </c>
       <c r="AM7" s="1">
-        <v>1.0793017642812827E-9</v>
+        <v>1.5845822624387198E-8</v>
       </c>
       <c r="AN7" s="1">
-        <v>1.5845822624387198E-8</v>
+        <v>1.1806091098449586E-8</v>
       </c>
       <c r="AO7" s="1">
-        <v>1.1806091098449586E-8</v>
+        <v>1.9685325094878723E-8</v>
       </c>
       <c r="AP7" s="1">
-        <v>1.9685325094878723E-8</v>
+        <v>1.4453969576777581E-8</v>
       </c>
       <c r="AQ7" s="1">
-        <v>1.4453969576777581E-8</v>
+        <v>7.0544436958641654E-10</v>
       </c>
       <c r="AR7" s="1">
-        <v>7.0544436958641654E-10</v>
+        <v>2.5023911740083525E-3</v>
       </c>
       <c r="AS7" s="1">
-        <v>-2.1115638126900649E-9</v>
+        <v>3.035488759531595E-3</v>
       </c>
       <c r="AT7" s="1">
-        <v>-4.9626770248778485E-8</v>
+        <v>0.97428977489471436</v>
       </c>
       <c r="AU7" s="1">
-        <v>2.5023911740083525E-3</v>
+        <v>0.903114914894104</v>
       </c>
       <c r="AV7" s="1">
-        <v>3.035488759531595E-3</v>
+        <v>0.79901474714279175</v>
       </c>
       <c r="AW7" s="1">
+        <v>0.67670148611068726</v>
+      </c>
+      <c r="AX7" s="1">
         <v>288</v>
-      </c>
-      <c r="AX7" s="1">
-        <v>1</v>
       </c>
       <c r="AY7" s="1">
         <v>1</v>
@@ -1475,43 +1488,43 @@
         <v>2.137178540806417E-7</v>
       </c>
       <c r="AL8" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>8.2776048450534965E-10</v>
       </c>
       <c r="AM8" s="1">
-        <v>8.2776048450534965E-10</v>
+        <v>1.3049375140815783E-8</v>
       </c>
       <c r="AN8" s="1">
-        <v>1.3049375140815783E-8</v>
+        <v>1.299671401077708E-8</v>
       </c>
       <c r="AO8" s="1">
-        <v>1.299671401077708E-8</v>
+        <v>2.1627551867085208E-8</v>
       </c>
       <c r="AP8" s="1">
-        <v>2.1627551867085208E-8</v>
+        <v>1.2962535045346613E-8</v>
       </c>
       <c r="AQ8" s="1">
-        <v>1.2962535045346613E-8</v>
+        <v>6.3265287453262431E-10</v>
       </c>
       <c r="AR8" s="1">
-        <v>6.3265287453262431E-10</v>
+        <v>2.7632727662240553E-3</v>
       </c>
       <c r="AS8" s="1">
-        <v>-2.2101518393213837E-9</v>
+        <v>3.825972231499949E-3</v>
       </c>
       <c r="AT8" s="1">
-        <v>-4.9192884432613937E-8</v>
+        <v>0.96431922912597656</v>
       </c>
       <c r="AU8" s="1">
-        <v>2.7632727662240553E-3</v>
+        <v>0.86854833364486694</v>
       </c>
       <c r="AV8" s="1">
-        <v>3.825972231499949E-3</v>
+        <v>0.7350771427154541</v>
       </c>
       <c r="AW8" s="1">
+        <v>0.58769595623016357</v>
+      </c>
+      <c r="AX8" s="1">
         <v>288</v>
-      </c>
-      <c r="AX8" s="1">
-        <v>1</v>
       </c>
       <c r="AY8" s="1">
         <v>1</v>
@@ -1672,43 +1685,43 @@
         <v>2.4767925310698047E-7</v>
       </c>
       <c r="AL9" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>6.2635599685405632E-10</v>
       </c>
       <c r="AM9" s="1">
-        <v>6.2635599685405632E-10</v>
+        <v>1.0230034916217332E-8</v>
       </c>
       <c r="AN9" s="1">
-        <v>1.0230034916217332E-8</v>
+        <v>1.4167870350761773E-8</v>
       </c>
       <c r="AO9" s="1">
-        <v>1.4167870350761773E-8</v>
+        <v>2.3526112730566477E-8</v>
       </c>
       <c r="AP9" s="1">
-        <v>2.3526112730566477E-8</v>
+        <v>1.14590292810135E-8</v>
       </c>
       <c r="AQ9" s="1">
-        <v>1.14590292810135E-8</v>
+        <v>5.592723506531172E-10</v>
       </c>
       <c r="AR9" s="1">
-        <v>5.592723506531172E-10</v>
+        <v>3.0068722737743147E-3</v>
       </c>
       <c r="AS9" s="1">
-        <v>-2.3209059119011499E-9</v>
+        <v>5.5830521753780886E-3</v>
       </c>
       <c r="AT9" s="1">
-        <v>-4.8311637357301151E-8</v>
+        <v>0.94568377733230591</v>
       </c>
       <c r="AU9" s="1">
-        <v>3.0068722737743147E-3</v>
+        <v>0.80802702903747559</v>
       </c>
       <c r="AV9" s="1">
-        <v>5.5830521753780886E-3</v>
+        <v>0.63216120004653931</v>
       </c>
       <c r="AW9" s="1">
+        <v>0.45789790153503418</v>
+      </c>
+      <c r="AX9" s="1">
         <v>288</v>
-      </c>
-      <c r="AX9" s="1">
-        <v>1</v>
       </c>
       <c r="AY9" s="1">
         <v>1</v>
@@ -1869,43 +1882,43 @@
         <v>2.6343693093622278E-7</v>
       </c>
       <c r="AL10" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>5.5126498836957378E-10</v>
       </c>
       <c r="AM10" s="1">
-        <v>5.5126498836957378E-10</v>
+        <v>8.4668842147087107E-9</v>
       </c>
       <c r="AN10" s="1">
-        <v>8.4668842147087107E-9</v>
+        <v>1.483114214382783E-8</v>
       </c>
       <c r="AO10" s="1">
-        <v>1.483114214382783E-8</v>
+        <v>2.4610872113796541E-8</v>
       </c>
       <c r="AP10" s="1">
-        <v>2.4610872113796541E-8</v>
+        <v>1.0733304023347046E-8</v>
       </c>
       <c r="AQ10" s="1">
-        <v>1.0733304023347046E-8</v>
+        <v>5.2385262794274468E-10</v>
       </c>
       <c r="AR10" s="1">
-        <v>5.2385262794274468E-10</v>
+        <v>3.1384469699312742E-3</v>
       </c>
       <c r="AS10" s="1">
-        <v>-2.3850339481157334E-9</v>
+        <v>8.1322923982073431E-3</v>
       </c>
       <c r="AT10" s="1">
-        <v>-4.7645684730923676E-8</v>
+        <v>0.92635989189147949</v>
       </c>
       <c r="AU10" s="1">
-        <v>3.1384469699312742E-3</v>
+        <v>0.75043618679046631</v>
       </c>
       <c r="AV10" s="1">
-        <v>8.1322923982073431E-3</v>
+        <v>0.54419207572937012</v>
       </c>
       <c r="AW10" s="1">
+        <v>0.35976284742355347</v>
+      </c>
+      <c r="AX10" s="1">
         <v>288</v>
-      </c>
-      <c r="AX10" s="1">
-        <v>1</v>
       </c>
       <c r="AY10" s="1">
         <v>1</v>
@@ -2066,43 +2079,43 @@
         <v>2.7411226710682968E-7</v>
       </c>
       <c r="AL11" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>5.3401148434451375E-10</v>
       </c>
       <c r="AM11" s="1">
-        <v>5.3401148434451375E-10</v>
+        <v>6.7408095631111472E-9</v>
       </c>
       <c r="AN11" s="1">
-        <v>6.7408095631111472E-9</v>
+        <v>1.5400749885444154E-8</v>
       </c>
       <c r="AO11" s="1">
-        <v>1.5400749885444154E-8</v>
+        <v>2.554980113784501E-8</v>
       </c>
       <c r="AP11" s="1">
-        <v>2.554980113784501E-8</v>
+        <v>1.0388052196219633E-8</v>
       </c>
       <c r="AQ11" s="1">
-        <v>1.0388052196219633E-8</v>
+        <v>5.0700194043074021E-10</v>
       </c>
       <c r="AR11" s="1">
-        <v>5.0700194043074021E-10</v>
+        <v>3.2669494528385534E-3</v>
       </c>
       <c r="AS11" s="1">
-        <v>-2.4518278518570469E-9</v>
+        <v>1.2870710287702493E-2</v>
       </c>
       <c r="AT11" s="1">
-        <v>-4.7142570736014022E-8</v>
+        <v>0.90161097049713135</v>
       </c>
       <c r="AU11" s="1">
-        <v>3.2669494528385534E-3</v>
+        <v>0.68356496095657349</v>
       </c>
       <c r="AV11" s="1">
-        <v>1.2870710287702493E-2</v>
+        <v>0.45325031876564026</v>
       </c>
       <c r="AW11" s="1">
+        <v>0.27036988735198975</v>
+      </c>
+      <c r="AX11" s="1">
         <v>288</v>
-      </c>
-      <c r="AX11" s="1">
-        <v>1</v>
       </c>
       <c r="AY11" s="1">
         <v>1</v>
@@ -2263,43 +2276,43 @@
         <v>2.8400916107784724E-7</v>
       </c>
       <c r="AL12" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>6.0408932910655379E-10</v>
       </c>
       <c r="AM12" s="1">
-        <v>6.0408932910655379E-10</v>
+        <v>4.4637916563133494E-9</v>
       </c>
       <c r="AN12" s="1">
-        <v>4.4637916563133494E-9</v>
+        <v>1.6079290233485255E-8</v>
       </c>
       <c r="AO12" s="1">
-        <v>1.6079290233485255E-8</v>
+        <v>2.6658059763991215E-8</v>
       </c>
       <c r="AP12" s="1">
-        <v>2.6658059763991215E-8</v>
+        <v>1.0517629434048104E-8</v>
       </c>
       <c r="AQ12" s="1">
-        <v>1.0517629434048104E-8</v>
+        <v>5.1332615935706372E-10</v>
       </c>
       <c r="AR12" s="1">
-        <v>5.1332615935706372E-10</v>
+        <v>3.5124426115541426E-3</v>
       </c>
       <c r="AS12" s="1">
-        <v>-2.5833812866693506E-9</v>
+        <v>2.6025033209277466E-2</v>
       </c>
       <c r="AT12" s="1">
-        <v>-4.6750415094720665E-8</v>
+        <v>0.85940617322921753</v>
       </c>
       <c r="AU12" s="1">
-        <v>3.5124426115541426E-3</v>
+        <v>0.58494079113006592</v>
       </c>
       <c r="AV12" s="1">
-        <v>2.6025033209277466E-2</v>
+        <v>0.33894208073616028</v>
       </c>
       <c r="AW12" s="1">
+        <v>0.17493276298046112</v>
+      </c>
+      <c r="AX12" s="1">
         <v>288</v>
-      </c>
-      <c r="AX12" s="1">
-        <v>1</v>
       </c>
       <c r="AY12" s="1">
         <v>1</v>
@@ -2460,43 +2473,43 @@
         <v>2.8937085971847409E-7</v>
       </c>
       <c r="AL13" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>7.4446952536890711E-10</v>
       </c>
       <c r="AM13" s="1">
-        <v>7.4446952536890711E-10</v>
+        <v>2.8981341774295476E-9</v>
       </c>
       <c r="AN13" s="1">
-        <v>2.8981341774295476E-9</v>
+        <v>1.6528485279228289E-8</v>
       </c>
       <c r="AO13" s="1">
-        <v>1.6528485279228289E-8</v>
+        <v>2.7364244936396026E-8</v>
       </c>
       <c r="AP13" s="1">
-        <v>2.7364244936396026E-8</v>
+        <v>1.1049430703735652E-8</v>
       </c>
       <c r="AQ13" s="1">
-        <v>1.1049430703735652E-8</v>
+        <v>5.3928134180480924E-10</v>
       </c>
       <c r="AR13" s="1">
-        <v>5.3928134180480924E-10</v>
+        <v>3.8356982014008654E-3</v>
       </c>
       <c r="AS13" s="1">
-        <v>-2.7278332925817494E-9</v>
+        <v>4.6414494448565109E-2</v>
       </c>
       <c r="AT13" s="1">
-        <v>-4.6521872576477108E-8</v>
+        <v>0.81981778144836426</v>
       </c>
       <c r="AU13" s="1">
-        <v>3.8356982014008654E-3</v>
+        <v>0.5072169303894043</v>
       </c>
       <c r="AV13" s="1">
-        <v>4.6414494448565109E-2</v>
+        <v>0.26369211077690125</v>
       </c>
       <c r="AW13" s="1">
+        <v>0.12218616157770157</v>
+      </c>
+      <c r="AX13" s="1">
         <v>288</v>
-      </c>
-      <c r="AX13" s="1">
-        <v>1</v>
       </c>
       <c r="AY13" s="1">
         <v>1</v>
@@ -2657,43 +2670,43 @@
         <v>2.5905802658598986E-7</v>
       </c>
       <c r="AL14" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>5.6894885978593483E-10</v>
       </c>
       <c r="AM14" s="1">
-        <v>5.6894885978593483E-10</v>
+        <v>9.0225432822009302E-9</v>
       </c>
       <c r="AN14" s="1">
-        <v>9.0225432822009302E-9</v>
+        <v>1.4631063248969622E-8</v>
       </c>
       <c r="AO14" s="1">
-        <v>1.4631063248969622E-8</v>
+        <v>2.4282343117254697E-8</v>
       </c>
       <c r="AP14" s="1">
-        <v>2.4282343117254697E-8</v>
+        <v>1.0925802484962333E-8</v>
       </c>
       <c r="AQ14" s="1">
-        <v>1.0925802484962333E-8</v>
+        <v>5.3324761273287891E-10</v>
       </c>
       <c r="AR14" s="1">
-        <v>5.3324761273287891E-10</v>
+        <v>3.0984529150511926E-3</v>
       </c>
       <c r="AS14" s="1">
-        <v>-2.3653179415106251E-9</v>
+        <v>7.1371250983980339E-3</v>
       </c>
       <c r="AT14" s="1">
-        <v>-4.7846359763070723E-8</v>
+        <v>0.93313455581665039</v>
       </c>
       <c r="AU14" s="1">
-        <v>3.0984529150511926E-3</v>
+        <v>0.77006024122238159</v>
       </c>
       <c r="AV14" s="1">
-        <v>7.1371250983980339E-3</v>
+        <v>0.57312440872192383</v>
       </c>
       <c r="AW14" s="1">
+        <v>0.39075762033462524</v>
+      </c>
+      <c r="AX14" s="1">
         <v>288</v>
-      </c>
-      <c r="AX14" s="1">
-        <v>1</v>
       </c>
       <c r="AY14" s="1">
         <v>1</v>
@@ -2854,43 +2867,43 @@
         <v>6.6366418138841254E-8</v>
       </c>
       <c r="AL15" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>2.862390786201319E-8</v>
       </c>
       <c r="AM15" s="1">
-        <v>2.862390786201319E-8</v>
+        <v>3.1560689468094732E-7</v>
       </c>
       <c r="AN15" s="1">
-        <v>3.1560689468094732E-7</v>
+        <v>7.5567457765574053E-7</v>
       </c>
       <c r="AO15" s="1">
-        <v>7.5567457765574053E-7</v>
+        <v>1.2529032601404921E-6</v>
       </c>
       <c r="AP15" s="1">
-        <v>1.2529032601404921E-6</v>
+        <v>5.5744044402672444E-7</v>
       </c>
       <c r="AQ15" s="1">
-        <v>5.5744044402672444E-7</v>
+        <v>2.7206585428984909E-8</v>
       </c>
       <c r="AR15" s="1">
-        <v>2.7206585428984909E-8</v>
+        <v>2.1130677782019327E-3</v>
       </c>
       <c r="AS15" s="1">
-        <v>-1.2282941952435067E-7</v>
+        <v>7.6243569005749866E-3</v>
       </c>
       <c r="AT15" s="1">
-        <v>-2.4601615677966038E-6</v>
+        <v>0.93315684795379639</v>
       </c>
       <c r="AU15" s="1">
-        <v>2.1130677782019327E-3</v>
+        <v>0.77012580633163452</v>
       </c>
       <c r="AV15" s="1">
-        <v>7.6243569005749866E-3</v>
+        <v>0.57322287559509277</v>
       </c>
       <c r="AW15" s="1">
+        <v>0.39086520671844482</v>
+      </c>
+      <c r="AX15" s="1">
         <v>288</v>
-      </c>
-      <c r="AX15" s="1">
-        <v>1</v>
       </c>
       <c r="AY15" s="1">
         <v>1</v>
@@ -3051,43 +3064,43 @@
         <v>1.8487964936753087E-8</v>
       </c>
       <c r="AL16" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>5.7675532828815885E-8</v>
       </c>
       <c r="AM16" s="1">
-        <v>5.7675532828815885E-8</v>
+        <v>3.9176351474045899E-7</v>
       </c>
       <c r="AN16" s="1">
-        <v>3.9176351474045899E-7</v>
+        <v>1.5561905789690522E-6</v>
       </c>
       <c r="AO16" s="1">
-        <v>1.5561905789690522E-6</v>
+        <v>2.5770099900540577E-6</v>
       </c>
       <c r="AP16" s="1">
-        <v>2.5770099900540577E-6</v>
+        <v>1.1352216233717627E-6</v>
       </c>
       <c r="AQ16" s="1">
-        <v>1.1352216233717627E-6</v>
+        <v>5.5405923404805435E-8</v>
       </c>
       <c r="AR16" s="1">
-        <v>5.5405923404805435E-8</v>
+        <v>1.1069586297016395E-3</v>
       </c>
       <c r="AS16" s="1">
-        <v>-2.5433195105506456E-7</v>
+        <v>8.1200806818931461E-3</v>
       </c>
       <c r="AT16" s="1">
-        <v>-5.0442436076991726E-6</v>
+        <v>0.93318110704421997</v>
       </c>
       <c r="AU16" s="1">
-        <v>1.1069586297016395E-3</v>
+        <v>0.77019709348678589</v>
       </c>
       <c r="AV16" s="1">
-        <v>8.1200806818931461E-3</v>
+        <v>0.57332992553710938</v>
       </c>
       <c r="AW16" s="1">
+        <v>0.3909822404384613</v>
+      </c>
+      <c r="AX16" s="1">
         <v>288</v>
-      </c>
-      <c r="AX16" s="1">
-        <v>1</v>
       </c>
       <c r="AY16" s="1">
         <v>1</v>
@@ -3248,43 +3261,43 @@
         <v>5.4320801190499424E-9</v>
       </c>
       <c r="AL17" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>1.1606258612083949E-7</v>
       </c>
       <c r="AM17" s="1">
-        <v>1.1606258612083949E-7</v>
+        <v>4.1252763651014492E-7</v>
       </c>
       <c r="AN17" s="1">
-        <v>4.1252763651014492E-7</v>
+        <v>3.1866778337219515E-6</v>
       </c>
       <c r="AO17" s="1">
-        <v>3.1866778337219515E-6</v>
+        <v>5.2665701475995697E-6</v>
       </c>
       <c r="AP17" s="1">
-        <v>5.2665701475995697E-6</v>
+        <v>2.3035370304569369E-6</v>
       </c>
       <c r="AQ17" s="1">
-        <v>2.3035370304569369E-6</v>
+        <v>1.1242703834568601E-7</v>
       </c>
       <c r="AR17" s="1">
-        <v>1.1242703834568601E-7</v>
+        <v>-9.0556657709961355E-4</v>
       </c>
       <c r="AS17" s="1">
-        <v>-5.2583595788746607E-7</v>
+        <v>9.1107622960835792E-3</v>
       </c>
       <c r="AT17" s="1">
-        <v>-1.0271794963045977E-5</v>
+        <v>0.93323057889938354</v>
       </c>
       <c r="AU17" s="1">
-        <v>-9.0556657709961355E-4</v>
+        <v>0.77034264802932739</v>
       </c>
       <c r="AV17" s="1">
-        <v>9.1107622960835792E-3</v>
+        <v>0.57354855537414551</v>
       </c>
       <c r="AW17" s="1">
+        <v>0.39122125506401062</v>
+      </c>
+      <c r="AX17" s="1">
         <v>288</v>
-      </c>
-      <c r="AX17" s="1">
-        <v>1</v>
       </c>
       <c r="AY17" s="1">
         <v>1</v>
@@ -3445,43 +3458,43 @@
         <v>1.4328112030170814E-9</v>
       </c>
       <c r="AL18" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>2.91729214505973E-7</v>
       </c>
       <c r="AM18" s="1">
-        <v>2.91729214505973E-7</v>
+        <v>4.1887792466901552E-7</v>
       </c>
       <c r="AN18" s="1">
-        <v>4.1887792466901552E-7</v>
+        <v>8.0962475287882363E-6</v>
       </c>
       <c r="AO18" s="1">
-        <v>8.0962475287882363E-6</v>
+        <v>1.3342353470280344E-5</v>
       </c>
       <c r="AP18" s="1">
-        <v>1.3342353470280344E-5</v>
+        <v>5.8377981986268423E-6</v>
       </c>
       <c r="AQ18" s="1">
-        <v>5.8377981986268423E-6</v>
+        <v>2.8492110004663118E-7</v>
       </c>
       <c r="AR18" s="1">
-        <v>2.8492110004663118E-7</v>
+        <v>-6.9428901325376121E-3</v>
       </c>
       <c r="AS18" s="1">
-        <v>-1.3543849490815774E-6</v>
+        <v>1.2082915985017321E-2</v>
       </c>
       <c r="AT18" s="1">
-        <v>-2.5965729946619831E-5</v>
+        <v>0.93337982892990112</v>
       </c>
       <c r="AU18" s="1">
-        <v>-6.9428901325376121E-3</v>
+        <v>0.77078181505203247</v>
       </c>
       <c r="AV18" s="1">
-        <v>1.2082915985017321E-2</v>
+        <v>0.57420849800109863</v>
       </c>
       <c r="AW18" s="1">
+        <v>0.39194324612617493</v>
+      </c>
+      <c r="AX18" s="1">
         <v>288</v>
-      </c>
-      <c r="AX18" s="1">
-        <v>1</v>
       </c>
       <c r="AY18" s="1">
         <v>1</v>
@@ -3642,43 +3655,43 @@
         <v>8.5186641074486147E-10</v>
       </c>
       <c r="AL19" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>4.3871460777547213E-7</v>
       </c>
       <c r="AM19" s="1">
-        <v>4.3871460777547213E-7</v>
+        <v>4.1980715758157299E-7</v>
       </c>
       <c r="AN19" s="1">
-        <v>4.1980715758157299E-7</v>
+        <v>1.218352345733198E-5</v>
       </c>
       <c r="AO19" s="1">
-        <v>1.218352345733198E-5</v>
+        <v>2.0060090131002184E-5</v>
       </c>
       <c r="AP19" s="1">
-        <v>2.0060090131002184E-5</v>
+        <v>8.8181013779831119E-6</v>
       </c>
       <c r="AQ19" s="1">
-        <v>8.8181013779831119E-6</v>
+        <v>4.3037854879912629E-7</v>
       </c>
       <c r="AR19" s="1">
-        <v>4.3037854879912629E-7</v>
+        <v>-1.1973685784724825E-2</v>
       </c>
       <c r="AS19" s="1">
-        <v>-2.0501295239228057E-6</v>
+        <v>1.4560062189143247E-2</v>
       </c>
       <c r="AT19" s="1">
-        <v>-3.9068920159479603E-5</v>
+        <v>0.93350446224212646</v>
       </c>
       <c r="AU19" s="1">
-        <v>-1.1973685784724825E-2</v>
+        <v>0.7711489200592041</v>
       </c>
       <c r="AV19" s="1">
-        <v>1.4560062189143247E-2</v>
+        <v>0.5747605562210083</v>
       </c>
       <c r="AW19" s="1">
+        <v>0.39254769682884216</v>
+      </c>
+      <c r="AX19" s="1">
         <v>288</v>
-      </c>
-      <c r="AX19" s="1">
-        <v>1</v>
       </c>
       <c r="AY19" s="1">
         <v>1</v>
@@ -3839,43 +3852,43 @@
         <v>5.9968596755055614E-10</v>
       </c>
       <c r="AL20" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>5.862725895224713E-7</v>
       </c>
       <c r="AM20" s="1">
-        <v>5.862725895224713E-7</v>
+        <v>4.2021107600448151E-7</v>
       </c>
       <c r="AN20" s="1">
-        <v>4.2021107600448151E-7</v>
+        <v>1.6262838366198906E-5</v>
       </c>
       <c r="AO20" s="1">
-        <v>1.6262838366198906E-5</v>
+        <v>2.6766246068232746E-5</v>
       </c>
       <c r="AP20" s="1">
-        <v>2.6766246068232746E-5</v>
+        <v>1.1832788914034609E-5</v>
       </c>
       <c r="AQ20" s="1">
-        <v>1.1832788914034609E-5</v>
+        <v>5.7751412896323018E-7</v>
       </c>
       <c r="AR20" s="1">
-        <v>5.7751412896323018E-7</v>
+        <v>-1.700429948106259E-2</v>
       </c>
       <c r="AS20" s="1">
-        <v>-2.748551423792378E-6</v>
+        <v>1.7037443932533262E-2</v>
       </c>
       <c r="AT20" s="1">
-        <v>-5.2204777603037655E-5</v>
+        <v>0.93362933397293091</v>
       </c>
       <c r="AU20" s="1">
-        <v>-1.700429948106259E-2</v>
+        <v>0.77151685953140259</v>
       </c>
       <c r="AV20" s="1">
-        <v>1.7037443932533262E-2</v>
+        <v>0.57531428337097168</v>
       </c>
       <c r="AW20" s="1">
+        <v>0.39315438270568848</v>
+      </c>
+      <c r="AX20" s="1">
         <v>288</v>
-      </c>
-      <c r="AX20" s="1">
-        <v>1</v>
       </c>
       <c r="AY20" s="1">
         <v>1</v>
@@ -4036,43 +4049,43 @@
         <v>3.7214589743150839E-10</v>
       </c>
       <c r="AL21" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>8.831254825368216E-7</v>
       </c>
       <c r="AM21" s="1">
-        <v>8.831254825368216E-7</v>
+        <v>4.205618508137978E-7</v>
       </c>
       <c r="AN21" s="1">
-        <v>4.205618508137978E-7</v>
+        <v>2.439233648021677E-5</v>
       </c>
       <c r="AO21" s="1">
-        <v>2.439233648021677E-5</v>
+        <v>4.0140446064595992E-5</v>
       </c>
       <c r="AP21" s="1">
-        <v>4.0140446064595992E-5</v>
+        <v>1.7968468455364928E-5</v>
       </c>
       <c r="AQ21" s="1">
-        <v>1.7968468455364928E-5</v>
+        <v>8.7697361550453934E-7</v>
       </c>
       <c r="AR21" s="1">
-        <v>8.7697361550453934E-7</v>
+        <v>-2.7065238867628762E-2</v>
       </c>
       <c r="AS21" s="1">
-        <v>-4.1522448555042502E-6</v>
+        <v>2.1992671739904601E-2</v>
       </c>
       <c r="AT21" s="1">
-        <v>-7.8586403105873615E-5</v>
+        <v>0.93387967348098755</v>
       </c>
       <c r="AU21" s="1">
-        <v>-2.7065238867628762E-2</v>
+        <v>0.77225512266159058</v>
       </c>
       <c r="AV21" s="1">
-        <v>2.1992671739904601E-2</v>
+        <v>0.57642638683319092</v>
       </c>
       <c r="AW21" s="1">
+        <v>0.39437434077262878</v>
+      </c>
+      <c r="AX21" s="1">
         <v>288</v>
-      </c>
-      <c r="AX21" s="1">
-        <v>1</v>
       </c>
       <c r="AY21" s="1">
         <v>1</v>
@@ -4233,43 +4246,43 @@
         <v>2.673633814342935E-10</v>
       </c>
       <c r="AL22" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>1.1822925471082456E-6</v>
       </c>
       <c r="AM22" s="1">
-        <v>1.1822925471082456E-6</v>
+        <v>4.2072620506857624E-7</v>
       </c>
       <c r="AN22" s="1">
-        <v>4.2072620506857624E-7</v>
+        <v>3.2479831417742133E-5</v>
       </c>
       <c r="AO22" s="1">
-        <v>3.2479831417742133E-5</v>
+        <v>5.3461060396831073E-5</v>
       </c>
       <c r="AP22" s="1">
-        <v>5.3461060396831073E-5</v>
+        <v>2.4251328795799054E-5</v>
       </c>
       <c r="AQ22" s="1">
-        <v>2.4251328795799054E-5</v>
+        <v>1.1836166322609643E-6</v>
       </c>
       <c r="AR22" s="1">
-        <v>1.1836166322609643E-6</v>
+        <v>-3.7126035358513082E-2</v>
       </c>
       <c r="AS22" s="1">
-        <v>-5.5648101806582417E-6</v>
+        <v>2.6948278474829661E-2</v>
       </c>
       <c r="AT22" s="1">
-        <v>-1.0512244625715539E-4</v>
+        <v>0.93413078784942627</v>
       </c>
       <c r="AU22" s="1">
-        <v>-3.7126035358513082E-2</v>
+        <v>0.77299642562866211</v>
       </c>
       <c r="AV22" s="1">
-        <v>2.6948278474829661E-2</v>
+        <v>0.57754462957382202</v>
       </c>
       <c r="AW22" s="1">
+        <v>0.39560288190841675</v>
+      </c>
+      <c r="AX22" s="1">
         <v>288</v>
-      </c>
-      <c r="AX22" s="1">
-        <v>1</v>
       </c>
       <c r="AY22" s="1">
         <v>1</v>
@@ -4430,43 +4443,43 @@
         <v>2.061236159534019E-8</v>
       </c>
       <c r="AL23" s="1">
-        <v>4.4979849705972796E-11</v>
+        <v>1.0398105565591158E-8</v>
       </c>
       <c r="AM23" s="1">
-        <v>1.0398105565591158E-8</v>
+        <v>5.8341632679611073E-10</v>
       </c>
       <c r="AN23" s="1">
-        <v>5.8341632679611073E-10</v>
+        <v>7.6069991021575993E-9</v>
       </c>
       <c r="AO23" s="1">
-        <v>7.6069991021575993E-9</v>
+        <v>1.2755204825832971E-8</v>
       </c>
       <c r="AP23" s="1">
-        <v>1.2755204825832971E-8</v>
+        <v>1.0528623306527152E-8</v>
       </c>
       <c r="AQ23" s="1">
-        <v>1.0528623306527152E-8</v>
+        <v>5.1386273014486505E-10</v>
       </c>
       <c r="AR23" s="1">
-        <v>5.1386273014486505E-10</v>
+        <v>1.2491880935093878E-3</v>
       </c>
       <c r="AS23" s="1">
-        <v>-1.6523592494266381E-9</v>
+        <v>3.6939247766086081E-3</v>
       </c>
       <c r="AT23" s="1">
-        <v>-4.2496669294678213E-8</v>
+        <v>0.93664896488189697</v>
       </c>
       <c r="AU23" s="1">
-        <v>1.2491880935093878E-3</v>
+        <v>0.78047728538513184</v>
       </c>
       <c r="AV23" s="1">
-        <v>3.6939247766086081E-3</v>
+        <v>0.58891528844833374</v>
       </c>
       <c r="AW23" s="1">
+        <v>0.40820139646530151</v>
+      </c>
+      <c r="AX23" s="1">
         <v>288</v>
-      </c>
-      <c r="AX23" s="1">
-        <v>1</v>
       </c>
       <c r="AY23" s="1">
         <v>1</v>
@@ -4627,43 +4640,43 @@
         <v>1.3885093608223542E-7</v>
       </c>
       <c r="AL24" s="1">
-        <v>4.4979850399862187E-10</v>
+        <v>9.4845825926188204E-9</v>
       </c>
       <c r="AM24" s="1">
-        <v>9.4845825926188204E-9</v>
+        <v>2.4211103541920192E-9</v>
       </c>
       <c r="AN24" s="1">
-        <v>2.4211103541920192E-9</v>
+        <v>1.1717371566049402E-8</v>
       </c>
       <c r="AO24" s="1">
-        <v>1.1717371566049402E-8</v>
+        <v>1.9562370966097079E-8</v>
       </c>
       <c r="AP24" s="1">
-        <v>1.9562370966097079E-8</v>
+        <v>1.1404772237710858E-8</v>
       </c>
       <c r="AQ24" s="1">
-        <v>1.1404772237710858E-8</v>
+        <v>5.5662424669478128E-10</v>
       </c>
       <c r="AR24" s="1">
-        <v>5.5662424669478128E-10</v>
+        <v>1.5256022555239059E-3</v>
       </c>
       <c r="AS24" s="1">
-        <v>-2.3521511405277806E-9</v>
+        <v>4.0761082626160038E-3</v>
       </c>
       <c r="AT24" s="1">
-        <v>-4.6177881074527249E-8</v>
+        <v>0.93688255548477173</v>
       </c>
       <c r="AU24" s="1">
-        <v>1.5256022555239059E-3</v>
+        <v>0.78117567300796509</v>
       </c>
       <c r="AV24" s="1">
-        <v>4.0761082626160038E-3</v>
+        <v>0.5899847149848938</v>
       </c>
       <c r="AW24" s="1">
+        <v>0.40939635038375854</v>
+      </c>
+      <c r="AX24" s="1">
         <v>288</v>
-      </c>
-      <c r="AX24" s="1">
-        <v>1</v>
       </c>
       <c r="AY24" s="1">
         <v>1</v>
@@ -4824,43 +4837,43 @@
         <v>3.2252543746835727E-7</v>
       </c>
       <c r="AL25" s="1">
-        <v>4.4979850954973699E-9</v>
+        <v>6.5943375775114749E-9</v>
       </c>
       <c r="AM25" s="1">
-        <v>6.5943375775114749E-9</v>
+        <v>4.9578719777426585E-9</v>
       </c>
       <c r="AN25" s="1">
-        <v>4.9578719777426585E-9</v>
+        <v>1.3766468189928182E-8</v>
       </c>
       <c r="AO25" s="1">
-        <v>1.3766468189928182E-8</v>
+        <v>2.2875949697994244E-8</v>
       </c>
       <c r="AP25" s="1">
-        <v>2.2875949697994244E-8</v>
+        <v>1.1206672034802523E-8</v>
       </c>
       <c r="AQ25" s="1">
-        <v>1.1206672034802523E-8</v>
+        <v>5.4695575846253064E-10</v>
       </c>
       <c r="AR25" s="1">
-        <v>5.4695575846253064E-10</v>
+        <v>2.3756143234378909E-3</v>
       </c>
       <c r="AS25" s="1">
-        <v>-2.397474885285078E-9</v>
+        <v>5.3504701995818645E-3</v>
       </c>
       <c r="AT25" s="1">
-        <v>-4.6222844218846149E-8</v>
+        <v>0.93581908941268921</v>
       </c>
       <c r="AU25" s="1">
-        <v>2.3756143234378909E-3</v>
+        <v>0.77800267934799194</v>
       </c>
       <c r="AV25" s="1">
-        <v>5.3504701995818645E-3</v>
+        <v>0.58513659238815308</v>
       </c>
       <c r="AW25" s="1">
+        <v>0.40399312973022461</v>
+      </c>
+      <c r="AX25" s="1">
         <v>288</v>
-      </c>
-      <c r="AX25" s="1">
-        <v>1</v>
       </c>
       <c r="AY25" s="1">
         <v>1</v>
@@ -5021,43 +5034,43 @@
         <v>3.3428815982006199E-7</v>
       </c>
       <c r="AL26" s="1">
-        <v>4.497984917861686E-8</v>
+        <v>1.692515486594569E-9</v>
       </c>
       <c r="AM26" s="1">
-        <v>1.692515486594569E-9</v>
+        <v>7.312585725378506E-9</v>
       </c>
       <c r="AN26" s="1">
-        <v>7.312585725378506E-9</v>
+        <v>1.4261458708799465E-8</v>
       </c>
       <c r="AO26" s="1">
-        <v>1.4261458708799465E-8</v>
+        <v>2.3670382844135892E-8</v>
       </c>
       <c r="AP26" s="1">
-        <v>2.3670382844135892E-8</v>
+        <v>1.0848707709953942E-8</v>
       </c>
       <c r="AQ26" s="1">
-        <v>1.0848707709953942E-8</v>
+        <v>5.2948484485781933E-10</v>
       </c>
       <c r="AR26" s="1">
-        <v>5.2948484485781933E-10</v>
+        <v>2.9410255973027193E-3</v>
       </c>
       <c r="AS26" s="1">
-        <v>-2.3680424288130553E-9</v>
+        <v>6.759722728174271E-3</v>
       </c>
       <c r="AT26" s="1">
-        <v>-4.6679179632747037E-8</v>
+        <v>0.93367773294448853</v>
       </c>
       <c r="AU26" s="1">
-        <v>2.9410255973027193E-3</v>
+        <v>0.77165943384170532</v>
       </c>
       <c r="AV26" s="1">
-        <v>6.759722728174271E-3</v>
+        <v>0.57552897930145264</v>
       </c>
       <c r="AW26" s="1">
+        <v>0.39338973164558411</v>
+      </c>
+      <c r="AX26" s="1">
         <v>288</v>
-      </c>
-      <c r="AX26" s="1">
-        <v>1</v>
       </c>
       <c r="AY26" s="1">
         <v>1</v>
@@ -5218,43 +5231,43 @@
         <v>1.6801651270270668E-7</v>
       </c>
       <c r="AL27" s="1">
-        <v>4.4979850599702331E-7</v>
+        <v>2.6246100323472354E-10</v>
       </c>
       <c r="AM27" s="1">
-        <v>2.6246100323472354E-10</v>
+        <v>1.0097348400122257E-8</v>
       </c>
       <c r="AN27" s="1">
-        <v>1.0097348400122257E-8</v>
+        <v>1.5080825523268448E-8</v>
       </c>
       <c r="AO27" s="1">
-        <v>1.5080825523268448E-8</v>
+        <v>2.5027419202610507E-8</v>
       </c>
       <c r="AP27" s="1">
-        <v>2.5027419202610507E-8</v>
+        <v>1.1120830478716925E-8</v>
       </c>
       <c r="AQ27" s="1">
-        <v>1.1120830478716925E-8</v>
+        <v>5.4276610983450269E-10</v>
       </c>
       <c r="AR27" s="1">
-        <v>5.4276610983450269E-10</v>
+        <v>3.1439506728161686E-3</v>
       </c>
       <c r="AS27" s="1">
-        <v>-2.3981083785429291E-9</v>
+        <v>7.2498701155968466E-3</v>
       </c>
       <c r="AT27" s="1">
-        <v>-4.9272994573357209E-8</v>
+        <v>0.9329717755317688</v>
       </c>
       <c r="AU27" s="1">
-        <v>3.1439506728161686E-3</v>
+        <v>0.76958161592483521</v>
       </c>
       <c r="AV27" s="1">
-        <v>7.2498701155968466E-3</v>
+        <v>0.57240617275238037</v>
       </c>
       <c r="AW27" s="1">
+        <v>0.38997307419776917</v>
+      </c>
+      <c r="AX27" s="1">
         <v>288</v>
-      </c>
-      <c r="AX27" s="1">
-        <v>1</v>
       </c>
       <c r="AY27" s="1">
         <v>1</v>
@@ -5415,43 +5428,43 @@
         <v>2.5246603030382175E-8</v>
       </c>
       <c r="AL28" s="1">
-        <v>4.4979851736570708E-6</v>
+        <v>8.7163037511199895E-11</v>
       </c>
       <c r="AM28" s="1">
-        <v>8.7163037511199895E-11</v>
+        <v>1.2125907891023076E-8</v>
       </c>
       <c r="AN28" s="1">
-        <v>1.2125907891023076E-8</v>
+        <v>1.6585499392277048E-8</v>
       </c>
       <c r="AO28" s="1">
-        <v>1.6585499392277048E-8</v>
+        <v>2.7674042727549031E-8</v>
       </c>
       <c r="AP28" s="1">
-        <v>2.7674042727549031E-8</v>
+        <v>1.1885022743740592E-8</v>
       </c>
       <c r="AQ28" s="1">
-        <v>1.1885022743740592E-8</v>
+        <v>5.8006349723527251E-10</v>
       </c>
       <c r="AR28" s="1">
-        <v>5.8006349723527251E-10</v>
+        <v>3.1137379871646982E-3</v>
       </c>
       <c r="AS28" s="1">
-        <v>-2.6187751966944006E-9</v>
+        <v>7.3390701579148137E-3</v>
       </c>
       <c r="AT28" s="1">
-        <v>-5.3969031910128251E-8</v>
+        <v>0.93269175291061401</v>
       </c>
       <c r="AU28" s="1">
-        <v>3.1137379871646982E-3</v>
+        <v>0.76875925064086914</v>
       </c>
       <c r="AV28" s="1">
-        <v>7.3390701579148137E-3</v>
+        <v>0.57117354869842529</v>
       </c>
       <c r="AW28" s="1">
+        <v>0.38862845301628113</v>
+      </c>
+      <c r="AX28" s="1">
         <v>288</v>
-      </c>
-      <c r="AX28" s="1">
-        <v>1</v>
       </c>
       <c r="AY28" s="1">
         <v>1</v>
@@ -5612,43 +5625,43 @@
         <v>1.2988572439809332E-9</v>
       </c>
       <c r="AL29" s="1">
-        <v>4.4979849917581305E-5</v>
+        <v>4.3744077920117292E-11</v>
       </c>
       <c r="AM29" s="1">
-        <v>4.3744077920117292E-11</v>
+        <v>1.4485365898694518E-8</v>
       </c>
       <c r="AN29" s="1">
-        <v>1.4485365898694518E-8</v>
+        <v>1.7436842197557367E-8</v>
       </c>
       <c r="AO29" s="1">
-        <v>1.7436842197557367E-8</v>
+        <v>3.0690675667521816E-8</v>
       </c>
       <c r="AP29" s="1">
-        <v>3.0690675667521816E-8</v>
+        <v>1.2929461945532239E-8</v>
       </c>
       <c r="AQ29" s="1">
-        <v>1.2929461945532239E-8</v>
+        <v>6.3103866576597056E-10</v>
       </c>
       <c r="AR29" s="1">
-        <v>6.3103866576597056E-10</v>
+        <v>2.7595461980379978E-3</v>
       </c>
       <c r="AS29" s="1">
-        <v>-2.8358366765957044E-9</v>
+        <v>7.5365753973853514E-3</v>
       </c>
       <c r="AT29" s="1">
-        <v>-5.8767312793861493E-8</v>
+        <v>0.93113869428634644</v>
       </c>
       <c r="AU29" s="1">
-        <v>2.7595461980379978E-3</v>
+        <v>0.76421678066253662</v>
       </c>
       <c r="AV29" s="1">
-        <v>7.5365753973853514E-3</v>
+        <v>0.56439882516860962</v>
       </c>
       <c r="AW29" s="1">
+        <v>0.38127866387367249</v>
+      </c>
+      <c r="AX29" s="1">
         <v>288</v>
-      </c>
-      <c r="AX29" s="1">
-        <v>1</v>
       </c>
       <c r="AY29" s="1">
         <v>1</v>
@@ -5809,43 +5822,43 @@
         <v>2.5680094495328376E-7</v>
       </c>
       <c r="AL30" s="1">
-        <v>5.0386113059630588E-8</v>
+        <v>6.5108985290349662E-10</v>
       </c>
       <c r="AM30" s="1">
-        <v>6.5108985290349662E-10</v>
+        <v>9.46897275793528E-9</v>
       </c>
       <c r="AN30" s="1">
-        <v>9.46897275793528E-9</v>
+        <v>1.4339961917995275E-8</v>
       </c>
       <c r="AO30" s="1">
-        <v>1.4339961917995275E-8</v>
+        <v>2.4105911040895028E-8</v>
       </c>
       <c r="AP30" s="1">
-        <v>2.4105911040895028E-8</v>
+        <v>1.0658757432224775E-8</v>
       </c>
       <c r="AQ30" s="1">
-        <v>1.0658757432224775E-8</v>
+        <v>5.2021409402414065E-10</v>
       </c>
       <c r="AR30" s="1">
-        <v>5.2021409402414065E-10</v>
+        <v>3.1148071807254054E-3</v>
       </c>
       <c r="AS30" s="1">
-        <v>-2.3170536600503056E-9</v>
+        <v>7.1865160025454695E-3</v>
       </c>
       <c r="AT30" s="1">
-        <v>-4.7161023530861712E-8</v>
+        <v>0.93423563241958618</v>
       </c>
       <c r="AU30" s="1">
-        <v>3.1148071807254054E-3</v>
+        <v>0.77355730533599854</v>
       </c>
       <c r="AV30" s="1">
-        <v>7.1865160025454695E-3</v>
+        <v>0.57877033948898315</v>
       </c>
       <c r="AW30" s="1">
+        <v>0.39736798405647278</v>
+      </c>
+      <c r="AX30" s="1">
         <v>274</v>
-      </c>
-      <c r="AX30" s="1">
-        <v>1</v>
       </c>
       <c r="AY30" s="1">
         <v>1</v>
@@ -6006,43 +6019,43 @@
         <v>2.5794932412281923E-7</v>
       </c>
       <c r="AL31" s="1">
-        <v>7.1851538052669639E-8</v>
+        <v>6.248171407347014E-10</v>
       </c>
       <c r="AM31" s="1">
-        <v>6.248171407347014E-10</v>
+        <v>9.3205768644424622E-9</v>
       </c>
       <c r="AN31" s="1">
-        <v>9.3205768644424622E-9</v>
+        <v>1.4414301038358224E-8</v>
       </c>
       <c r="AO31" s="1">
-        <v>1.4414301038358224E-8</v>
+        <v>2.4154820491440604E-8</v>
       </c>
       <c r="AP31" s="1">
-        <v>2.4154820491440604E-8</v>
+        <v>1.0728481214528074E-8</v>
       </c>
       <c r="AQ31" s="1">
-        <v>1.0728481214528074E-8</v>
+        <v>5.2361703861691922E-10</v>
       </c>
       <c r="AR31" s="1">
-        <v>5.2361703861691922E-10</v>
+        <v>3.1098493988407534E-3</v>
       </c>
       <c r="AS31" s="1">
-        <v>-2.3298341034205805E-9</v>
+        <v>7.173630456403424E-3</v>
       </c>
       <c r="AT31" s="1">
-        <v>-4.7339916875444032E-8</v>
+        <v>0.93391072750091553</v>
       </c>
       <c r="AU31" s="1">
-        <v>3.1098493988407534E-3</v>
+        <v>0.77252644300460815</v>
       </c>
       <c r="AV31" s="1">
-        <v>7.173630456403424E-3</v>
+        <v>0.57710623741149902</v>
       </c>
       <c r="AW31" s="1">
+        <v>0.39541810750961304</v>
+      </c>
+      <c r="AX31" s="1">
         <v>278</v>
-      </c>
-      <c r="AX31" s="1">
-        <v>1</v>
       </c>
       <c r="AY31" s="1">
         <v>1</v>
@@ -6203,43 +6216,43 @@
         <v>2.5883386456371227E-7</v>
       </c>
       <c r="AL32" s="1">
-        <v>1.1039902858556161E-7</v>
+        <v>5.952485073856123E-10</v>
       </c>
       <c r="AM32" s="1">
-        <v>5.952485073856123E-10</v>
+        <v>9.1571212176030084E-9</v>
       </c>
       <c r="AN32" s="1">
-        <v>9.1571212176030084E-9</v>
+        <v>1.4516749084173171E-8</v>
       </c>
       <c r="AO32" s="1">
-        <v>1.4516749084173171E-8</v>
+        <v>2.4217216888951232E-8</v>
       </c>
       <c r="AP32" s="1">
-        <v>2.4217216888951232E-8</v>
+        <v>1.0822861717940668E-8</v>
       </c>
       <c r="AQ32" s="1">
-        <v>1.0822861717940668E-8</v>
+        <v>5.2822335394608899E-10</v>
       </c>
       <c r="AR32" s="1">
-        <v>5.2822335394608899E-10</v>
+        <v>3.1039915447911284E-3</v>
       </c>
       <c r="AS32" s="1">
-        <v>-2.3467738863303111E-9</v>
+        <v>7.156130876253157E-3</v>
       </c>
       <c r="AT32" s="1">
-        <v>-4.758155114359397E-8</v>
+        <v>0.93351620435714722</v>
       </c>
       <c r="AU32" s="1">
-        <v>3.1039915447911284E-3</v>
+        <v>0.77127355337142944</v>
       </c>
       <c r="AV32" s="1">
-        <v>7.156130876253157E-3</v>
+        <v>0.57508355379104614</v>
       </c>
       <c r="AW32" s="1">
+        <v>0.39304983615875244</v>
+      </c>
+      <c r="AX32" s="1">
         <v>283</v>
-      </c>
-      <c r="AX32" s="1">
-        <v>1</v>
       </c>
       <c r="AY32" s="1">
         <v>1</v>
@@ -6400,43 +6413,43 @@
         <v>2.5905774236889556E-7</v>
       </c>
       <c r="AL33" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>5.6895281758465033E-10</v>
       </c>
       <c r="AM33" s="1">
-        <v>5.6895281758465033E-10</v>
+        <v>9.0225792038986964E-9</v>
       </c>
       <c r="AN33" s="1">
-        <v>9.0225792038986964E-9</v>
+        <v>1.4631477221319945E-8</v>
       </c>
       <c r="AO33" s="1">
-        <v>1.4631477221319945E-8</v>
+        <v>2.4283039289432762E-8</v>
       </c>
       <c r="AP33" s="1">
-        <v>2.4283039289432762E-8</v>
+        <v>1.0926068050309823E-8</v>
       </c>
       <c r="AQ33" s="1">
-        <v>1.0926068050309823E-8</v>
+        <v>5.3326054683111579E-10</v>
       </c>
       <c r="AR33" s="1">
-        <v>5.3326054683111579E-10</v>
+        <v>3.0984529692265898E-3</v>
       </c>
       <c r="AS33" s="1">
-        <v>-2.3653181635552301E-9</v>
+        <v>7.1371251514870228E-3</v>
       </c>
       <c r="AT33" s="1">
-        <v>-4.7847176887216847E-8</v>
+        <v>0.93313455581665039</v>
       </c>
       <c r="AU33" s="1">
-        <v>3.0984529692265898E-3</v>
+        <v>0.77006024122238159</v>
       </c>
       <c r="AV33" s="1">
-        <v>7.1371251514870228E-3</v>
+        <v>0.57312440872192383</v>
       </c>
       <c r="AW33" s="1">
+        <v>0.39075762033462524</v>
+      </c>
+      <c r="AX33" s="1">
         <v>288</v>
-      </c>
-      <c r="AX33" s="1">
-        <v>1</v>
       </c>
       <c r="AY33" s="1">
         <v>1</v>
@@ -6597,43 +6610,43 @@
         <v>2.5853290708255372E-7</v>
       </c>
       <c r="AL34" s="1">
-        <v>2.4941655851762334E-7</v>
+        <v>5.4557986844646147E-10</v>
       </c>
       <c r="AM34" s="1">
-        <v>5.4557986844646147E-10</v>
+        <v>8.9220320198626619E-9</v>
       </c>
       <c r="AN34" s="1">
-        <v>8.9220320198626619E-9</v>
+        <v>1.4759921008176448E-8</v>
       </c>
       <c r="AO34" s="1">
-        <v>1.4759921008176448E-8</v>
+        <v>2.4353866790415013E-8</v>
       </c>
       <c r="AP34" s="1">
-        <v>2.4353866790415013E-8</v>
+        <v>1.103874502916824E-8</v>
       </c>
       <c r="AQ34" s="1">
-        <v>1.103874502916824E-8</v>
+        <v>5.3875987005014281E-10</v>
       </c>
       <c r="AR34" s="1">
-        <v>5.3875987005014281E-10</v>
+        <v>3.0931885314652357E-3</v>
       </c>
       <c r="AS34" s="1">
-        <v>-2.3860471376480064E-9</v>
+        <v>7.1166596089337125E-3</v>
       </c>
       <c r="AT34" s="1">
-        <v>-4.8139835229221717E-8</v>
+        <v>0.93276584148406982</v>
       </c>
       <c r="AU34" s="1">
-        <v>3.0931885314652357E-3</v>
+        <v>0.7688862681388855</v>
       </c>
       <c r="AV34" s="1">
-        <v>7.1166596089337125E-3</v>
+        <v>0.5712282657623291</v>
       </c>
       <c r="AW34" s="1">
+        <v>0.38854023814201355</v>
+      </c>
+      <c r="AX34" s="1">
         <v>293</v>
-      </c>
-      <c r="AX34" s="1">
-        <v>1</v>
       </c>
       <c r="AY34" s="1">
         <v>1</v>
@@ -6794,43 +6807,43 @@
         <v>2.5712898832352948E-7</v>
       </c>
       <c r="AL35" s="1">
-        <v>3.6727897168020718E-7</v>
+        <v>5.2481405828671938E-10</v>
       </c>
       <c r="AM35" s="1">
-        <v>5.2481405828671938E-10</v>
+        <v>8.8600900077142551E-9</v>
       </c>
       <c r="AN35" s="1">
-        <v>8.8600900077142551E-9</v>
+        <v>1.4902400140509933E-8</v>
       </c>
       <c r="AO35" s="1">
-        <v>1.4902400140509933E-8</v>
+        <v>2.4429472522810233E-8</v>
       </c>
       <c r="AP35" s="1">
-        <v>2.4429472522810233E-8</v>
+        <v>1.1160876667304365E-8</v>
       </c>
       <c r="AQ35" s="1">
-        <v>1.1160876667304365E-8</v>
+        <v>5.4472060195820404E-10</v>
       </c>
       <c r="AR35" s="1">
-        <v>5.4472060195820404E-10</v>
+        <v>3.0881496887887449E-3</v>
       </c>
       <c r="AS35" s="1">
-        <v>-2.4094830575194237E-9</v>
+        <v>7.0947942592767006E-3</v>
       </c>
       <c r="AT35" s="1">
-        <v>-4.8459224188945882E-8</v>
+        <v>0.93240982294082642</v>
       </c>
       <c r="AU35" s="1">
-        <v>3.0881496887887449E-3</v>
+        <v>0.76775115728378296</v>
       </c>
       <c r="AV35" s="1">
-        <v>7.0947942592767006E-3</v>
+        <v>0.56939399242401123</v>
       </c>
       <c r="AW35" s="1">
+        <v>0.38639608025550842</v>
+      </c>
+      <c r="AX35" s="1">
         <v>298</v>
-      </c>
-      <c r="AX35" s="1">
-        <v>1</v>
       </c>
       <c r="AY35" s="1">
         <v>1</v>
@@ -6991,43 +7004,43 @@
         <v>1.2209516730976588E-9</v>
       </c>
       <c r="AL36" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>1.0852616299551762E-7</v>
       </c>
       <c r="AM36" s="1">
-        <v>1.0852616299551762E-7</v>
+        <v>4.183657516475821E-7</v>
       </c>
       <c r="AN36" s="1">
-        <v>4.183657516475821E-7</v>
+        <v>1.4185524507930036E-6</v>
       </c>
       <c r="AO36" s="1">
-        <v>1.4185524507930036E-6</v>
+        <v>2.3501101289909176E-6</v>
       </c>
       <c r="AP36" s="1">
-        <v>2.3501101289909176E-6</v>
+        <v>1.5558740642518387E-6</v>
       </c>
       <c r="AQ36" s="1">
-        <v>1.5558740642518387E-6</v>
+        <v>7.5936426924272382E-8</v>
       </c>
       <c r="AR36" s="1">
-        <v>7.5936426924272382E-8</v>
+        <v>4.8752561467802673E-4</v>
       </c>
       <c r="AS36" s="1">
-        <v>-2.5621042709644826E-7</v>
+        <v>4.0169389923219983E-3</v>
       </c>
       <c r="AT36" s="1">
-        <v>-5.4653723964293022E-6</v>
+        <v>0.97440832853317261</v>
       </c>
       <c r="AU36" s="1">
-        <v>4.8752561467802673E-4</v>
+        <v>0.90353554487228394</v>
       </c>
       <c r="AV36" s="1">
-        <v>4.0169389923219983E-3</v>
+        <v>0.79981696605682373</v>
       </c>
       <c r="AW36" s="1">
+        <v>0.67785972356796265</v>
+      </c>
+      <c r="AX36" s="1">
         <v>288</v>
-      </c>
-      <c r="AX36" s="1">
-        <v>1</v>
       </c>
       <c r="AY36" s="1">
         <v>1</v>
@@ -7188,43 +7201,43 @@
         <v>3.1481290907464654E-9</v>
       </c>
       <c r="AL37" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>8.3707256060688877E-8</v>
       </c>
       <c r="AM37" s="1">
-        <v>8.3707256060688877E-8</v>
+        <v>4.1516866560213789E-7</v>
       </c>
       <c r="AN37" s="1">
-        <v>4.1516866560213789E-7</v>
+        <v>1.4706404143083329E-6</v>
       </c>
       <c r="AO37" s="1">
-        <v>1.4706404143083329E-6</v>
+        <v>2.4358894233911244E-6</v>
       </c>
       <c r="AP37" s="1">
-        <v>2.4358894233911244E-6</v>
+        <v>1.3758934755969676E-6</v>
       </c>
       <c r="AQ37" s="1">
-        <v>1.3758934755969676E-6</v>
+        <v>6.7152221561173064E-8</v>
       </c>
       <c r="AR37" s="1">
-        <v>6.7152221561173064E-8</v>
+        <v>7.6585490419767447E-4</v>
       </c>
       <c r="AS37" s="1">
-        <v>-2.5466687247899245E-7</v>
+        <v>4.8107019868062857E-3</v>
       </c>
       <c r="AT37" s="1">
-        <v>-5.3202797971607652E-6</v>
+        <v>0.96441179513931274</v>
       </c>
       <c r="AU37" s="1">
-        <v>7.6585490419767447E-4</v>
+        <v>0.86886215209960938</v>
       </c>
       <c r="AV37" s="1">
-        <v>4.8107019868062857E-3</v>
+        <v>0.73564034700393677</v>
       </c>
       <c r="AW37" s="1">
+        <v>0.58845162391662598</v>
+      </c>
+      <c r="AX37" s="1">
         <v>288</v>
-      </c>
-      <c r="AX37" s="1">
-        <v>1</v>
       </c>
       <c r="AY37" s="1">
         <v>1</v>
@@ -7385,43 +7398,43 @@
         <v>1.0436821185066947E-8</v>
       </c>
       <c r="AL38" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>6.3479242803227143E-8</v>
       </c>
       <c r="AM38" s="1">
-        <v>6.3479242803227143E-8</v>
+        <v>4.0386055056309893E-7</v>
       </c>
       <c r="AN38" s="1">
-        <v>4.0386055056309893E-7</v>
+        <v>1.5297625433619011E-6</v>
       </c>
       <c r="AO38" s="1">
-        <v>1.5297625433619011E-6</v>
+        <v>2.5334123965187194E-6</v>
       </c>
       <c r="AP38" s="1">
-        <v>2.5334123965187194E-6</v>
+        <v>1.1983946706095594E-6</v>
       </c>
       <c r="AQ38" s="1">
-        <v>1.1983946706095594E-6</v>
+        <v>5.8489153076379807E-8</v>
       </c>
       <c r="AR38" s="1">
-        <v>5.8489153076379807E-8</v>
+        <v>1.0145536559166175E-3</v>
       </c>
       <c r="AS38" s="1">
-        <v>-2.5387871005477791E-7</v>
+        <v>6.5662035609586333E-3</v>
       </c>
       <c r="AT38" s="1">
-        <v>-5.1342444749025162E-6</v>
+        <v>0.94574403762817383</v>
       </c>
       <c r="AU38" s="1">
-        <v>1.0145536559166175E-3</v>
+        <v>0.80821460485458374</v>
       </c>
       <c r="AV38" s="1">
-        <v>6.5662035609586333E-3</v>
+        <v>0.63246321678161621</v>
       </c>
       <c r="AW38" s="1">
+        <v>0.45825493335723877</v>
+      </c>
+      <c r="AX38" s="1">
         <v>288</v>
-      </c>
-      <c r="AX38" s="1">
-        <v>1</v>
       </c>
       <c r="AY38" s="1">
         <v>1</v>
@@ -7582,43 +7595,43 @@
         <v>2.3894120459999613E-8</v>
       </c>
       <c r="AL39" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>5.5878355793154151E-8</v>
       </c>
       <c r="AM39" s="1">
-        <v>5.5878355793154151E-8</v>
+        <v>3.8373821727822641E-7</v>
       </c>
       <c r="AN39" s="1">
-        <v>3.8373821727822641E-7</v>
+        <v>1.5680852317595528E-6</v>
       </c>
       <c r="AO39" s="1">
-        <v>1.5680852317595528E-6</v>
+        <v>2.5966141058847425E-6</v>
       </c>
       <c r="AP39" s="1">
-        <v>2.5966141058847425E-6</v>
+        <v>1.1118974043711205E-6</v>
       </c>
       <c r="AQ39" s="1">
-        <v>1.1118974043711205E-6</v>
+        <v>5.4267566440557857E-8</v>
       </c>
       <c r="AR39" s="1">
-        <v>5.4267566440557857E-8</v>
+        <v>1.1472220484468592E-3</v>
       </c>
       <c r="AS39" s="1">
-        <v>-2.5483362264822063E-7</v>
+        <v>9.1152954847186721E-3</v>
       </c>
       <c r="AT39" s="1">
-        <v>-5.0035923777613789E-6</v>
+        <v>0.92640066146850586</v>
       </c>
       <c r="AU39" s="1">
-        <v>1.1472220484468592E-3</v>
+        <v>0.75055265426635742</v>
       </c>
       <c r="AV39" s="1">
-        <v>9.1152954847186721E-3</v>
+        <v>0.5443606972694397</v>
       </c>
       <c r="AW39" s="1">
+        <v>0.35993984341621399</v>
+      </c>
+      <c r="AX39" s="1">
         <v>288</v>
-      </c>
-      <c r="AX39" s="1">
-        <v>1</v>
       </c>
       <c r="AY39" s="1">
         <v>1</v>
@@ -7779,43 +7792,43 @@
         <v>4.9048662020823031E-8</v>
       </c>
       <c r="AL40" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>5.406338348008799E-8</v>
       </c>
       <c r="AM40" s="1">
-        <v>5.406338348008799E-8</v>
+        <v>3.4701382584706173E-7</v>
       </c>
       <c r="AN40" s="1">
-        <v>3.4701382584706173E-7</v>
+        <v>1.6026292241622109E-6</v>
       </c>
       <c r="AO40" s="1">
-        <v>1.6026292241622109E-6</v>
+        <v>2.6533014374496844E-6</v>
       </c>
       <c r="AP40" s="1">
-        <v>2.6533014374496844E-6</v>
+        <v>1.0661287888069637E-6</v>
       </c>
       <c r="AQ40" s="1">
-        <v>1.0661287888069637E-6</v>
+        <v>5.2033747977020539E-8</v>
       </c>
       <c r="AR40" s="1">
-        <v>5.2033747977020539E-8</v>
+        <v>1.2763079053072378E-3</v>
       </c>
       <c r="AS40" s="1">
-        <v>-2.5792752467168611E-7</v>
+        <v>1.3854174876868377E-2</v>
       </c>
       <c r="AT40" s="1">
-        <v>-4.8885995056480169E-6</v>
+        <v>0.90163719654083252</v>
       </c>
       <c r="AU40" s="1">
-        <v>1.2763079053072378E-3</v>
+        <v>0.68363213539123535</v>
       </c>
       <c r="AV40" s="1">
-        <v>1.3854174876868377E-2</v>
+        <v>0.4533359706401825</v>
       </c>
       <c r="AW40" s="1">
+        <v>0.27044841647148132</v>
+      </c>
+      <c r="AX40" s="1">
         <v>288</v>
-      </c>
-      <c r="AX40" s="1">
-        <v>1</v>
       </c>
       <c r="AY40" s="1">
         <v>1</v>
@@ -7976,43 +7989,43 @@
         <v>1.0305642916819124E-7</v>
       </c>
       <c r="AL41" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>6.091680330609292E-8</v>
       </c>
       <c r="AM41" s="1">
-        <v>6.091680330609292E-8</v>
+        <v>2.6996251910852805E-7</v>
       </c>
       <c r="AN41" s="1">
-        <v>2.6996251910852805E-7</v>
+        <v>1.6446263312874798E-6</v>
       </c>
       <c r="AO41" s="1">
-        <v>1.6446263312874798E-6</v>
+        <v>2.7208790590871335E-6</v>
       </c>
       <c r="AP41" s="1">
-        <v>2.7208790590871335E-6</v>
+        <v>1.0666167327144649E-6</v>
       </c>
       <c r="AQ41" s="1">
-        <v>1.0666167327144649E-6</v>
+        <v>5.2057572474950575E-8</v>
       </c>
       <c r="AR41" s="1">
-        <v>5.2057572474950575E-8</v>
+        <v>1.5221696712095375E-3</v>
       </c>
       <c r="AS41" s="1">
-        <v>-2.6668746500035923E-7</v>
+        <v>2.7009327548093619E-2</v>
       </c>
       <c r="AT41" s="1">
-        <v>-4.7670728235971183E-6</v>
+        <v>0.85941970348358154</v>
       </c>
       <c r="AU41" s="1">
-        <v>1.5221696712095375E-3</v>
+        <v>0.58496969938278198</v>
       </c>
       <c r="AV41" s="1">
-        <v>2.7009327548093619E-2</v>
+        <v>0.33897235989570618</v>
       </c>
       <c r="AW41" s="1">
+        <v>0.17495560646057129</v>
+      </c>
+      <c r="AX41" s="1">
         <v>288</v>
-      </c>
-      <c r="AX41" s="1">
-        <v>1</v>
       </c>
       <c r="AY41" s="1">
         <v>1</v>
@@ -8173,43 +8186,43 @@
         <v>1.5442310541402549E-7</v>
       </c>
       <c r="AL42" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>7.4795844752810134E-8</v>
       </c>
       <c r="AM42" s="1">
-        <v>7.4795844752810134E-8</v>
+        <v>1.9794738796789774E-7</v>
       </c>
       <c r="AN42" s="1">
-        <v>1.9794738796789774E-7</v>
+        <v>1.6735200709661058E-6</v>
       </c>
       <c r="AO42" s="1">
-        <v>1.6735200709661058E-6</v>
+        <v>2.7655472825127703E-6</v>
       </c>
       <c r="AP42" s="1">
-        <v>2.7655472825127703E-6</v>
+        <v>1.1125849823656608E-6</v>
       </c>
       <c r="AQ42" s="1">
-        <v>1.1125849823656608E-6</v>
+        <v>5.4301107610399413E-8</v>
       </c>
       <c r="AR42" s="1">
-        <v>5.4301107610399413E-8</v>
+        <v>1.8455365637069909E-3</v>
       </c>
       <c r="AS42" s="1">
-        <v>-2.7771901045525738E-7</v>
+        <v>4.7399451577391179E-2</v>
       </c>
       <c r="AT42" s="1">
-        <v>-4.6963991735538002E-6</v>
+        <v>0.81982553005218506</v>
       </c>
       <c r="AU42" s="1">
-        <v>1.8455365637069909E-3</v>
+        <v>0.50723087787628174</v>
       </c>
       <c r="AV42" s="1">
-        <v>4.7399451577391179E-2</v>
+        <v>0.26370453834533691</v>
       </c>
       <c r="AW42" s="1">
+        <v>0.12219421565532684</v>
+      </c>
+      <c r="AX42" s="1">
         <v>288</v>
-      </c>
-      <c r="AX42" s="1">
-        <v>1</v>
       </c>
       <c r="AY42" s="1">
         <v>1</v>
@@ -8370,43 +8383,43 @@
         <v>1.810232674870349E-8</v>
       </c>
       <c r="AL43" s="1">
-        <v>4.4979849705972796E-11</v>
+        <v>1.039410845549843E-6</v>
       </c>
       <c r="AM43" s="1">
-        <v>1.039410845549843E-6</v>
+        <v>5.1953401638667905E-8</v>
       </c>
       <c r="AN43" s="1">
-        <v>5.1953401638667905E-8</v>
+        <v>7.61771361369951E-7</v>
       </c>
       <c r="AO43" s="1">
-        <v>7.61771361369951E-7</v>
+        <v>1.2773193446459246E-6</v>
       </c>
       <c r="AP43" s="1">
-        <v>1.2773193446459246E-6</v>
+        <v>1.0534571401876747E-6</v>
       </c>
       <c r="AQ43" s="1">
-        <v>1.0534571401876747E-6</v>
+        <v>5.1415302237955984E-8</v>
       </c>
       <c r="AR43" s="1">
-        <v>5.1415302237955984E-8</v>
+        <v>-7.371304861770755E-4</v>
       </c>
       <c r="AS43" s="1">
-        <v>-1.6531390656382428E-7</v>
+        <v>4.6795887204886793E-3</v>
       </c>
       <c r="AT43" s="1">
-        <v>-4.2519600356172305E-6</v>
+        <v>0.93667101860046387</v>
       </c>
       <c r="AU43" s="1">
-        <v>-7.371304861770755E-4</v>
+        <v>0.78054326772689819</v>
       </c>
       <c r="AV43" s="1">
-        <v>4.6795887204886793E-3</v>
+        <v>0.58901619911193848</v>
       </c>
       <c r="AW43" s="1">
+        <v>0.40831413865089417</v>
+      </c>
+      <c r="AX43" s="1">
         <v>288</v>
-      </c>
-      <c r="AX43" s="1">
-        <v>1</v>
       </c>
       <c r="AY43" s="1">
         <v>1</v>
@@ -8567,43 +8580,43 @@
         <v>8.473807611153461E-8</v>
       </c>
       <c r="AL44" s="1">
-        <v>4.4979850399862187E-10</v>
+        <v>9.4957947287949152E-7</v>
       </c>
       <c r="AM44" s="1">
-        <v>9.4957947287949152E-7</v>
+        <v>1.6573201911716401E-7</v>
       </c>
       <c r="AN44" s="1">
-        <v>1.6573201911716401E-7</v>
+        <v>1.1842633701431085E-6</v>
       </c>
       <c r="AO44" s="1">
-        <v>1.1842633701431085E-6</v>
+        <v>1.9764400214719444E-6</v>
       </c>
       <c r="AP44" s="1">
-        <v>1.9764400214719444E-6</v>
+        <v>1.1450317742855987E-6</v>
       </c>
       <c r="AQ44" s="1">
-        <v>1.1450317742855987E-6</v>
+        <v>5.5884722627297378E-8</v>
       </c>
       <c r="AR44" s="1">
-        <v>5.5884722627297378E-8</v>
+        <v>-4.7229598000750843E-4</v>
       </c>
       <c r="AS44" s="1">
-        <v>-2.3985225539036037E-7</v>
+        <v>5.0510324479078623E-3</v>
       </c>
       <c r="AT44" s="1">
-        <v>-4.6351615310413763E-6</v>
+        <v>0.93692123889923096</v>
       </c>
       <c r="AU44" s="1">
-        <v>-4.7229598000750843E-4</v>
+        <v>0.78129136562347412</v>
       </c>
       <c r="AV44" s="1">
-        <v>5.0510324479078623E-3</v>
+        <v>0.59016209840774536</v>
       </c>
       <c r="AW44" s="1">
+        <v>0.40959468483924866</v>
+      </c>
+      <c r="AX44" s="1">
         <v>288</v>
-      </c>
-      <c r="AX44" s="1">
-        <v>1</v>
       </c>
       <c r="AY44" s="1">
         <v>1</v>
@@ -8764,43 +8777,43 @@
         <v>1.0565872088363903E-7</v>
       </c>
       <c r="AL45" s="1">
-        <v>4.4979850954973699E-9</v>
+        <v>6.6322111041267062E-7</v>
       </c>
       <c r="AM45" s="1">
-        <v>6.6322111041267062E-7</v>
+        <v>2.8489269851998463E-7</v>
       </c>
       <c r="AN45" s="1">
-        <v>2.8489269851998463E-7</v>
+        <v>1.4132458037620236E-6</v>
       </c>
       <c r="AO45" s="1">
-        <v>1.4132458037620236E-6</v>
+        <v>2.3457964679898195E-6</v>
       </c>
       <c r="AP45" s="1">
-        <v>2.3457964679898195E-6</v>
+        <v>1.1374683026588173E-6</v>
       </c>
       <c r="AQ45" s="1">
-        <v>1.1374683026588173E-6</v>
+        <v>5.5515581465215291E-8</v>
       </c>
       <c r="AR45" s="1">
-        <v>5.5515581465215291E-8</v>
+        <v>3.7287308713088071E-4</v>
       </c>
       <c r="AS45" s="1">
-        <v>-2.499622553386871E-7</v>
+        <v>6.3213803935189333E-3</v>
       </c>
       <c r="AT45" s="1">
-        <v>-4.7087742132134736E-6</v>
+        <v>0.93586510419845581</v>
       </c>
       <c r="AU45" s="1">
-        <v>3.7287308713088071E-4</v>
+        <v>0.77813959121704102</v>
       </c>
       <c r="AV45" s="1">
-        <v>6.3213803935189333E-3</v>
+        <v>0.58534520864486694</v>
       </c>
       <c r="AW45" s="1">
+        <v>0.40422490239143372</v>
+      </c>
+      <c r="AX45" s="1">
         <v>288</v>
-      </c>
-      <c r="AX45" s="1">
-        <v>1</v>
       </c>
       <c r="AY45" s="1">
         <v>1</v>
@@ -8961,43 +8974,43 @@
         <v>4.6087048843901357E-8</v>
       </c>
       <c r="AL46" s="1">
-        <v>4.497984917861686E-8</v>
+        <v>1.7112754369802419E-7</v>
       </c>
       <c r="AM46" s="1">
-        <v>1.7112754369802419E-7</v>
+        <v>3.6413202624361457E-7</v>
       </c>
       <c r="AN46" s="1">
-        <v>3.6413202624361457E-7</v>
+        <v>1.4933970201407021E-6</v>
       </c>
       <c r="AO46" s="1">
-        <v>1.4933970201407021E-6</v>
+        <v>2.4752200749530995E-6</v>
       </c>
       <c r="AP46" s="1">
-        <v>2.4752200749530995E-6</v>
+        <v>1.1173843859069166E-6</v>
       </c>
       <c r="AQ46" s="1">
-        <v>1.1173843859069166E-6</v>
+        <v>5.4535355786811124E-8</v>
       </c>
       <c r="AR46" s="1">
-        <v>5.4535355786811124E-8</v>
+        <v>9.4492897864416716E-4</v>
       </c>
       <c r="AS46" s="1">
-        <v>-2.5148895588245068E-7</v>
+        <v>7.7379574022964212E-3</v>
       </c>
       <c r="AT46" s="1">
-        <v>-4.8580168368062004E-6</v>
+        <v>0.93372339010238647</v>
       </c>
       <c r="AU46" s="1">
-        <v>9.4492897864416716E-4</v>
+        <v>0.77179414033889771</v>
       </c>
       <c r="AV46" s="1">
-        <v>7.7379574022964212E-3</v>
+        <v>0.57573181390762329</v>
       </c>
       <c r="AW46" s="1">
+        <v>0.39361217617988586</v>
+      </c>
+      <c r="AX46" s="1">
         <v>288</v>
-      </c>
-      <c r="AX46" s="1">
-        <v>1</v>
       </c>
       <c r="AY46" s="1">
         <v>1</v>
@@ -9158,43 +9171,43 @@
         <v>8.1458466638650862E-9</v>
       </c>
       <c r="AL47" s="1">
-        <v>4.4979850599702331E-7</v>
+        <v>2.6638046440527477E-8</v>
       </c>
       <c r="AM47" s="1">
-        <v>2.6638046440527477E-8</v>
+        <v>4.0123879271493517E-7</v>
       </c>
       <c r="AN47" s="1">
-        <v>4.0123879271493517E-7</v>
+        <v>1.614937308630493E-6</v>
       </c>
       <c r="AO47" s="1">
-        <v>1.614937308630493E-6</v>
+        <v>2.6702815567603011E-6</v>
       </c>
       <c r="AP47" s="1">
-        <v>2.6702815567603011E-6</v>
+        <v>1.1565533668544958E-6</v>
       </c>
       <c r="AQ47" s="1">
-        <v>1.1565533668544958E-6</v>
+        <v>5.6447053253805279E-8</v>
       </c>
       <c r="AR47" s="1">
-        <v>5.6447053253805279E-8</v>
+        <v>1.1535871840948448E-3</v>
       </c>
       <c r="AS47" s="1">
-        <v>-2.5818081894612988E-7</v>
+        <v>8.2337945752603784E-3</v>
       </c>
       <c r="AT47" s="1">
-        <v>-5.2024802243977319E-6</v>
+        <v>0.93301945924758911</v>
       </c>
       <c r="AU47" s="1">
-        <v>1.1535871840948448E-3</v>
+        <v>0.76972180604934692</v>
       </c>
       <c r="AV47" s="1">
-        <v>8.2337945752603784E-3</v>
+        <v>0.5726165771484375</v>
       </c>
       <c r="AW47" s="1">
+        <v>0.39020279049873352</v>
+      </c>
+      <c r="AX47" s="1">
         <v>288</v>
-      </c>
-      <c r="AX47" s="1">
-        <v>1</v>
       </c>
       <c r="AY47" s="1">
         <v>1</v>
@@ -9355,43 +9368,43 @@
         <v>7.3798700483962421E-10</v>
       </c>
       <c r="AL48" s="1">
-        <v>4.4979851736570708E-6</v>
+        <v>8.8174946274565541E-9</v>
       </c>
       <c r="AM48" s="1">
-        <v>8.8174946274565541E-9</v>
+        <v>4.0919967703498561E-7</v>
       </c>
       <c r="AN48" s="1">
-        <v>4.0919967703498561E-7</v>
+        <v>1.7746335758683784E-6</v>
       </c>
       <c r="AO48" s="1">
-        <v>1.7746335758683784E-6</v>
+        <v>2.9296702779291195E-6</v>
       </c>
       <c r="AP48" s="1">
-        <v>2.9296702779291195E-6</v>
+        <v>1.2126946558055351E-6</v>
       </c>
       <c r="AQ48" s="1">
-        <v>1.2126946558055351E-6</v>
+        <v>5.9187087231293845E-8</v>
       </c>
       <c r="AR48" s="1">
-        <v>5.9187087231293845E-8</v>
+        <v>1.1229346720723523E-3</v>
       </c>
       <c r="AS48" s="1">
-        <v>-2.6569929900688294E-7</v>
+        <v>8.3223293811068456E-3</v>
       </c>
       <c r="AT48" s="1">
-        <v>-5.5457053349527996E-6</v>
+        <v>0.93274253606796265</v>
       </c>
       <c r="AU48" s="1">
-        <v>1.1229346720723523E-3</v>
+        <v>0.76890832185745239</v>
       </c>
       <c r="AV48" s="1">
-        <v>8.3223293811068456E-3</v>
+        <v>0.57139688730239868</v>
       </c>
       <c r="AW48" s="1">
+        <v>0.38887187838554382</v>
+      </c>
+      <c r="AX48" s="1">
         <v>288</v>
-      </c>
-      <c r="AX48" s="1">
-        <v>1</v>
       </c>
       <c r="AY48" s="1">
         <v>1</v>
@@ -9552,43 +9565,43 @@
         <v>2.9408184221146882E-11</v>
       </c>
       <c r="AL49" s="1">
-        <v>4.4979849917581305E-5</v>
+        <v>4.3835715982120695E-9</v>
       </c>
       <c r="AM49" s="1">
-        <v>4.3835715982120695E-9</v>
+        <v>4.1195969622466681E-7</v>
       </c>
       <c r="AN49" s="1">
-        <v>4.1195969622466681E-7</v>
+        <v>1.8808077916210308E-6</v>
       </c>
       <c r="AO49" s="1">
-        <v>1.8808077916210308E-6</v>
+        <v>3.26474084832995E-6</v>
       </c>
       <c r="AP49" s="1">
-        <v>3.26474084832995E-6</v>
+        <v>1.3013127500016708E-6</v>
       </c>
       <c r="AQ49" s="1">
-        <v>1.3013127500016708E-6</v>
+        <v>6.3512210601857078E-8</v>
       </c>
       <c r="AR49" s="1">
-        <v>6.3512210601857078E-8</v>
+        <v>7.6808612075729692E-4</v>
       </c>
       <c r="AS49" s="1">
-        <v>-2.6943556008518499E-7</v>
+        <v>8.5202269591933937E-3</v>
       </c>
       <c r="AT49" s="1">
-        <v>-5.923292974330252E-6</v>
+        <v>0.93118423223495483</v>
       </c>
       <c r="AU49" s="1">
-        <v>7.6808612075729692E-4</v>
+        <v>0.76434963941574097</v>
       </c>
       <c r="AV49" s="1">
-        <v>8.5202269591933937E-3</v>
+        <v>0.56459617614746094</v>
       </c>
       <c r="AW49" s="1">
+        <v>0.38149181008338928</v>
+      </c>
+      <c r="AX49" s="1">
         <v>288</v>
-      </c>
-      <c r="AX49" s="1">
-        <v>1</v>
       </c>
       <c r="AY49" s="1">
         <v>1</v>
@@ -9749,43 +9762,43 @@
         <v>1.4944971482577785E-8</v>
       </c>
       <c r="AL50" s="1">
-        <v>5.0386113059630588E-8</v>
+        <v>6.6204596560134887E-8</v>
       </c>
       <c r="AM50" s="1">
-        <v>6.6204596560134887E-8</v>
+        <v>3.9720876133042141E-7</v>
       </c>
       <c r="AN50" s="1">
-        <v>3.9720876133042141E-7</v>
+        <v>1.5405814329863543E-6</v>
       </c>
       <c r="AO50" s="1">
-        <v>1.5405814329863543E-6</v>
+        <v>2.5835288706768655E-6</v>
       </c>
       <c r="AP50" s="1">
-        <v>2.5835288706768655E-6</v>
+        <v>1.1145443750137929E-6</v>
       </c>
       <c r="AQ50" s="1">
-        <v>1.1145443750137929E-6</v>
+        <v>5.4396746662632722E-8</v>
       </c>
       <c r="AR50" s="1">
-        <v>5.4396746662632722E-8</v>
+        <v>1.1238568601179692E-3</v>
       </c>
       <c r="AS50" s="1">
-        <v>-2.5221413579856744E-7</v>
+        <v>8.1700843285073717E-3</v>
       </c>
       <c r="AT50" s="1">
-        <v>-5.0178014134871773E-6</v>
+        <v>0.93428242206573486</v>
       </c>
       <c r="AU50" s="1">
-        <v>1.1238568601179692E-3</v>
+        <v>0.77369523048400879</v>
       </c>
       <c r="AV50" s="1">
-        <v>8.1700843285073717E-3</v>
+        <v>0.57897841930389404</v>
       </c>
       <c r="AW50" s="1">
+        <v>0.39759686589241028</v>
+      </c>
+      <c r="AX50" s="1">
         <v>274</v>
-      </c>
-      <c r="AX50" s="1">
-        <v>1</v>
       </c>
       <c r="AY50" s="1">
         <v>1</v>
@@ -9946,43 +9959,43 @@
         <v>1.6051993512178342E-8</v>
       </c>
       <c r="AL51" s="1">
-        <v>7.1851538052669639E-8</v>
+        <v>6.3480456212808289E-8</v>
       </c>
       <c r="AM51" s="1">
-        <v>6.3480456212808289E-8</v>
+        <v>3.9554587605126253E-7</v>
       </c>
       <c r="AN51" s="1">
-        <v>3.9554587605126253E-7</v>
+        <v>1.5442351513419994E-6</v>
       </c>
       <c r="AO51" s="1">
-        <v>1.5442351513419994E-6</v>
+        <v>2.5816992413607576E-6</v>
       </c>
       <c r="AP51" s="1">
-        <v>2.5816992413607576E-6</v>
+        <v>1.1198925449207309E-6</v>
       </c>
       <c r="AQ51" s="1">
-        <v>1.1198925449207309E-6</v>
+        <v>5.4657760983900516E-8</v>
       </c>
       <c r="AR51" s="1">
-        <v>5.4657760983900516E-8</v>
+        <v>1.1187283702755939E-3</v>
       </c>
       <c r="AS51" s="1">
-        <v>-2.5269363845836779E-7</v>
+        <v>8.1569931342962889E-3</v>
       </c>
       <c r="AT51" s="1">
-        <v>-5.0243038458575029E-6</v>
+        <v>0.93395745754241943</v>
       </c>
       <c r="AU51" s="1">
-        <v>1.1187283702755939E-3</v>
+        <v>0.77266407012939453</v>
       </c>
       <c r="AV51" s="1">
-        <v>8.1569931342962889E-3</v>
+        <v>0.57731354236602783</v>
       </c>
       <c r="AW51" s="1">
+        <v>0.39564573764801025</v>
+      </c>
+      <c r="AX51" s="1">
         <v>278</v>
-      </c>
-      <c r="AX51" s="1">
-        <v>1</v>
       </c>
       <c r="AY51" s="1">
         <v>1</v>
@@ -10143,43 +10156,43 @@
         <v>1.7351450054547968E-8</v>
       </c>
       <c r="AL52" s="1">
-        <v>1.1039902858556161E-7</v>
+        <v>6.0411027380177784E-8</v>
       </c>
       <c r="AM52" s="1">
-        <v>6.0411027380177784E-8</v>
+        <v>3.9355082448417774E-7</v>
       </c>
       <c r="AN52" s="1">
-        <v>3.9355082448417774E-7</v>
+        <v>1.5497199496034009E-6</v>
       </c>
       <c r="AO52" s="1">
-        <v>1.5497199496034009E-6</v>
+        <v>2.5794144350305137E-6</v>
       </c>
       <c r="AP52" s="1">
-        <v>2.5794144350305137E-6</v>
+        <v>1.127223754338047E-6</v>
       </c>
       <c r="AQ52" s="1">
-        <v>1.127223754338047E-6</v>
+        <v>5.5015576094774588E-8</v>
       </c>
       <c r="AR52" s="1">
-        <v>5.5015576094774588E-8</v>
+        <v>1.1126735678306365E-3</v>
       </c>
       <c r="AS52" s="1">
-        <v>-2.5342274057038594E-7</v>
+        <v>8.1392734645958659E-3</v>
       </c>
       <c r="AT52" s="1">
-        <v>-5.0335570449533407E-6</v>
+        <v>0.93356281518936157</v>
       </c>
       <c r="AU52" s="1">
-        <v>1.1126735678306365E-3</v>
+        <v>0.77141082286834717</v>
       </c>
       <c r="AV52" s="1">
-        <v>8.1392734645958659E-3</v>
+        <v>0.57528996467590332</v>
       </c>
       <c r="AW52" s="1">
+        <v>0.39327597618103027</v>
+      </c>
+      <c r="AX52" s="1">
         <v>283</v>
-      </c>
-      <c r="AX52" s="1">
-        <v>1</v>
       </c>
       <c r="AY52" s="1">
         <v>1</v>
@@ -10340,43 +10353,43 @@
         <v>1.8487964936753087E-8</v>
       </c>
       <c r="AL53" s="1">
-        <v>1.6711598505025904E-7</v>
+        <v>5.7675532828815885E-8</v>
       </c>
       <c r="AM53" s="1">
-        <v>5.7675532828815885E-8</v>
+        <v>3.9176351474045899E-7</v>
       </c>
       <c r="AN53" s="1">
-        <v>3.9176351474045899E-7</v>
+        <v>1.5561905789690522E-6</v>
       </c>
       <c r="AO53" s="1">
-        <v>1.5561905789690522E-6</v>
+        <v>2.5770099900540577E-6</v>
       </c>
       <c r="AP53" s="1">
-        <v>2.5770099900540577E-6</v>
+        <v>1.1352216233717627E-6</v>
       </c>
       <c r="AQ53" s="1">
-        <v>1.1352216233717627E-6</v>
+        <v>5.5405923404805435E-8</v>
       </c>
       <c r="AR53" s="1">
-        <v>5.5405923404805435E-8</v>
+        <v>1.1069586301759315E-3</v>
       </c>
       <c r="AS53" s="1">
-        <v>-2.5433195105506456E-7</v>
+        <v>8.1200806814626363E-3</v>
       </c>
       <c r="AT53" s="1">
-        <v>-5.0442436076991726E-6</v>
+        <v>0.93318110704421997</v>
       </c>
       <c r="AU53" s="1">
-        <v>1.1069586301759315E-3</v>
+        <v>0.77019709348678589</v>
       </c>
       <c r="AV53" s="1">
-        <v>8.1200806814626363E-3</v>
+        <v>0.57332992553710938</v>
       </c>
       <c r="AW53" s="1">
+        <v>0.3909822404384613</v>
+      </c>
+      <c r="AX53" s="1">
         <v>288</v>
-      </c>
-      <c r="AX53" s="1">
-        <v>1</v>
       </c>
       <c r="AY53" s="1">
         <v>1</v>
@@ -10537,43 +10550,43 @@
         <v>1.937315907696302E-8</v>
       </c>
       <c r="AL54" s="1">
-        <v>2.4941655851762334E-7</v>
+        <v>5.5238297909723795E-8</v>
       </c>
       <c r="AM54" s="1">
-        <v>5.5238297909723795E-8</v>
+        <v>3.9028106891014842E-7</v>
       </c>
       <c r="AN54" s="1">
-        <v>3.9028106891014842E-7</v>
+        <v>1.5639020537056014E-6</v>
       </c>
       <c r="AO54" s="1">
-        <v>1.5639020537056014E-6</v>
+        <v>2.57485223947862E-6</v>
       </c>
       <c r="AP54" s="1">
-        <v>2.57485223947862E-6</v>
+        <v>1.1440396292528021E-6</v>
       </c>
       <c r="AQ54" s="1">
-        <v>1.1440396292528021E-6</v>
+        <v>5.5836295587141649E-8</v>
       </c>
       <c r="AR54" s="1">
-        <v>5.5836295587141649E-8</v>
+        <v>1.1015286039247872E-3</v>
       </c>
       <c r="AS54" s="1">
-        <v>-2.5546404458509642E-7</v>
+        <v>8.099457408802007E-3</v>
       </c>
       <c r="AT54" s="1">
-        <v>-5.0565754463605117E-6</v>
+        <v>0.93281227350234985</v>
       </c>
       <c r="AU54" s="1">
-        <v>1.1015286039247872E-3</v>
+        <v>0.76902276277542114</v>
       </c>
       <c r="AV54" s="1">
-        <v>8.099457408802007E-3</v>
+        <v>0.57143288850784302</v>
       </c>
       <c r="AW54" s="1">
+        <v>0.38876339793205261</v>
+      </c>
+      <c r="AX54" s="1">
         <v>293</v>
-      </c>
-      <c r="AX54" s="1">
-        <v>1</v>
       </c>
       <c r="AY54" s="1">
         <v>1</v>
@@ -10734,43 +10747,43 @@
         <v>1.9921785110454948E-8</v>
       </c>
       <c r="AL55" s="1">
-        <v>3.6727897168020718E-7</v>
+        <v>5.3067108114063239E-8</v>
       </c>
       <c r="AM55" s="1">
-        <v>5.3067108114063239E-8</v>
+        <v>3.8923465716031883E-7</v>
       </c>
       <c r="AN55" s="1">
-        <v>3.8923465716031883E-7</v>
+        <v>1.5728806264381223E-6</v>
       </c>
       <c r="AO55" s="1">
-        <v>1.5728806264381223E-6</v>
+        <v>2.5729332538693139E-6</v>
       </c>
       <c r="AP55" s="1">
-        <v>2.5729332538693139E-6</v>
+        <v>1.1536811825862969E-6</v>
       </c>
       <c r="AQ55" s="1">
-        <v>1.1536811825862969E-6</v>
+        <v>5.6306873830180848E-8</v>
       </c>
       <c r="AR55" s="1">
-        <v>5.6306873830180848E-8</v>
+        <v>1.0963356103017526E-3</v>
       </c>
       <c r="AS55" s="1">
-        <v>-2.5685477567094495E-7</v>
+        <v>8.0774562067730173E-3</v>
       </c>
       <c r="AT55" s="1">
-        <v>-5.0706016736512538E-6</v>
+        <v>0.93245619535446167</v>
       </c>
       <c r="AU55" s="1">
-        <v>1.0963356103017526E-3</v>
+        <v>0.76788729429244995</v>
       </c>
       <c r="AV55" s="1">
-        <v>8.0774562067730173E-3</v>
+        <v>0.56959778070449829</v>
       </c>
       <c r="AW55" s="1">
+        <v>0.38661786913871765</v>
+      </c>
+      <c r="AX55" s="1">
         <v>298</v>
-      </c>
-      <c r="AX55" s="1">
-        <v>1</v>
       </c>
       <c r="AY55" s="1">
         <v>1</v>
@@ -10822,8 +10835,8 @@
   <printOptions gridLines="1"/>
   <pageMargins left="1.5" right="1.5" top="1.5" bottom="1.5" header="0.5" footer="0.5"/>
   <headerFooter>
-    <oddHeader>BLM version Ver 3.57.2.50, build 2023-06-15</oddHeader>
-    <oddFooter>BLM Output File, C:\Users\kellyc\Documents\BLM Development\engine\BLMEngineInR\scrap\old BLM\full_organic.det.xls, created 01-31-2024</oddFooter>
+    <oddHeader>BLM version Ver 3.57.2.45, build 2021-04-05</oddHeader>
+    <oddFooter>BLM Output File, C:\Users\kellyc\Documents\BLM Development\engine\BLMEngineInR\scrap\old BLM\full_organic.det.xls, created 03-05-2024</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>